<commit_message>
Update Test Case for Gone Sin Mal.xlsx
</commit_message>
<xml_diff>
--- a/Bit Geeks - Project/Gone Sin Mal (Testing)/Test Case for Gone Sin Mal.xlsx
+++ b/Bit Geeks - Project/Gone Sin Mal (Testing)/Test Case for Gone Sin Mal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gone_Sin_Mal\Final_GoneSinMal\Bit-Geek-Project-Documents-\Bit Geeks - Project\Gone Sin Mal (Testing)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE1A3B9-7245-4E80-855D-6A62C98163E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6D294C-5160-4413-B48B-4FC6F6DB02AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6910" activeTab="2" xr2:uid="{0C18B1CA-7377-4DAD-81F8-23E85DEB025F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6910" xr2:uid="{0C18B1CA-7377-4DAD-81F8-23E85DEB025F}"/>
   </bookViews>
   <sheets>
     <sheet name="Restaurant Side" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="184">
   <si>
     <t xml:space="preserve">Title </t>
   </si>
@@ -637,6 +637,9 @@
   <si>
     <t>Enter correct username and correct password 
 and click "Login" button</t>
+  </si>
+  <si>
+    <t>Reported by YUNE NADI OO</t>
   </si>
 </sst>
 </file>
@@ -699,7 +702,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -722,11 +725,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -830,6 +842,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3F5A57-EEC8-43F9-B21A-F15755916C0B}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1163,83 +1178,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+    <row r="4" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>10</v>
@@ -1256,200 +1251,200 @@
     </row>
     <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
+    <row r="12" spans="1:8" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
         <v>1</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10">
+      <c r="E12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10">
         <v>2</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
+      <c r="E13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
         <v>3</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
+      <c r="E14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
-        <v>5</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>31</v>
@@ -1470,71 +1465,71 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
+        <v>5</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
         <v>6</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
+      <c r="E17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
         <v>7</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A18" s="9">
-        <v>8</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="E18" s="6" t="s">
         <v>24</v>
       </c>
@@ -1542,24 +1537,24 @@
         <v>11</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>8</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>24</v>
@@ -1574,110 +1569,110 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5">
-        <v>10</v>
+    <row r="20" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="9">
+        <v>8</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
+        <v>10</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="12" t="s">
+      <c r="F21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="H21" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-    </row>
-    <row r="23" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
-        <v>1</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>24</v>
@@ -1694,16 +1689,16 @@
     </row>
     <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>24</v>
@@ -1720,16 +1715,16 @@
     </row>
     <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>24</v>
@@ -1744,119 +1739,119 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="6">
+        <v>4</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="5">
+    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="5">
         <v>1</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="5">
+      <c r="E32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="5">
         <v>2</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="12" t="s">
+      <c r="E33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="5">
-        <v>3</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>13</v>
@@ -1864,68 +1859,68 @@
     </row>
     <row r="34" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
+        <v>3</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="5">
         <v>4</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="12" t="s">
+      <c r="E35" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H34" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="15">
+      <c r="H35" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="15">
         <v>5</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D36" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="15">
-        <v>6</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>10</v>
@@ -1942,108 +1937,108 @@
     </row>
     <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="15">
+        <v>7</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+      <c r="E38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-    </row>
-    <row r="40" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H41" s="4" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="5">
-        <v>1</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>31</v>
+        <v>125</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>24</v>
@@ -2060,10 +2055,10 @@
     </row>
     <row r="43" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>31</v>
@@ -2071,7 +2066,7 @@
       <c r="D43" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F43" s="9" t="s">
@@ -2086,68 +2081,68 @@
     </row>
     <row r="44" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
+        <v>3</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="5">
         <v>4</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B45" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E44" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="15">
+      <c r="E45" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="15">
         <v>5</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B46" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="15">
-        <v>6</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>24</v>
@@ -2162,234 +2157,234 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
+        <v>6</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="15">
         <v>7</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B48" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C48" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D48" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E47" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+      <c r="E48" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-    </row>
-    <row r="50" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="4" t="s">
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+    </row>
+    <row r="51" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="G51" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="H51" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="5">
+    <row r="52" spans="1:8" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="5">
         <v>1</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B52" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="5">
+      <c r="E52" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="5">
         <v>2</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B53" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C53" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E52" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="5">
+      <c r="E53" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5">
         <v>3</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B54" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C54" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D54" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E53" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="5">
+      <c r="E54" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="5">
         <v>4</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E54" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="6" t="s">
+      <c r="E55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G54" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="15">
+      <c r="G55" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="15">
         <v>5</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B56" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E55" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" s="15">
+      <c r="E56" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="15">
         <v>6</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" s="26">
-        <v>7</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>139</v>
@@ -2397,25 +2392,25 @@
       <c r="D57" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="5">
-        <v>8</v>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="26">
+        <v>7</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>139</v>
@@ -2423,25 +2418,25 @@
       <c r="D58" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G58" s="12" t="s">
-        <v>144</v>
+      <c r="G58" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="15">
-        <v>9</v>
+      <c r="A59" s="5">
+        <v>8</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>139</v>
@@ -2449,185 +2444,185 @@
       <c r="D59" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E59" s="18" t="s">
+      <c r="E59" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="8" t="s">
-        <v>12</v>
+      <c r="G59" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="H59" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60" s="20"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="22"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+    <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="15">
+        <v>9</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="20"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="22"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-    </row>
-    <row r="66" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="4" t="s">
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+    </row>
+    <row r="67" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E67" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="F67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="G67" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="4" t="s">
+      <c r="H67" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="5">
+    <row r="68" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="5">
         <v>1</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B68" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C68" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D68" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E67" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="5">
+      <c r="E68" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="5">
         <v>2</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B69" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C69" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D69" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E68" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G68" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H68" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="10">
+      <c r="E69" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="10">
         <v>3</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B70" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C70" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="D70" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E69" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G69" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H69" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="24">
+      <c r="E70" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="24">
         <v>4</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B71" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C71" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D70" s="10" t="s">
+      <c r="D71" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="E70" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H70" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" s="5">
-        <v>5</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>10</v>
@@ -2647,7 +2642,7 @@
         <v>5</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>146</v>
@@ -2669,12 +2664,41 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B73" s="25"/>
+      <c r="A73" s="5">
+        <v>5</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B74" s="25"/>
     </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B75" s="25"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2790,7 +2814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -2816,7 +2840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2876,7 +2900,7 @@
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
     </row>
-    <row r="10" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -2902,7 +2926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="174" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>1</v>
       </c>
@@ -2928,7 +2952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>2</v>
       </c>
@@ -2954,7 +2978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>3</v>
       </c>
@@ -2980,7 +3004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>4</v>
       </c>
@@ -3006,7 +3030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>5</v>
       </c>
@@ -3032,7 +3056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>6</v>
       </c>
@@ -3058,7 +3082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>7</v>
       </c>
@@ -3110,7 +3134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="145" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>9</v>
       </c>
@@ -3136,7 +3160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>10</v>
       </c>
@@ -3162,7 +3186,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="174" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>11</v>
       </c>
@@ -3249,7 +3273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAAA496-E45D-49E8-82B3-2109E613F4ED}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>